<commit_message>
Endurance Surface Piercing Profiler Cal and Ingest CSV update
changes to Endurance Surface Piercing Profiler Cal amnd INgest sheets

Reference designator corrections
Lat Lon formats
Removing m from depth value
</commit_message>
<xml_diff>
--- a/CE06ISSP/Omaha_Cal_Info_CE06ISSP_00002.xlsx
+++ b/CE06ISSP/Omaha_Cal_Info_CE06ISSP_00002.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\CE06ISSP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="885" yWindow="975" windowWidth="25605" windowHeight="16065" tabRatio="579"/>
+    <workbookView xWindow="885" yWindow="975" windowWidth="25605" windowHeight="16065" tabRatio="579" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -21,7 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Asset_Cal_Info!$A$1:$G$51</definedName>
     <definedName name="Workbook1" localSheetId="1">Asset_Cal_Info!$F$5:$F$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2289,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,8 +2306,8 @@
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="18.28515625" customWidth="1"/>
@@ -2494,13 +2499,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>